<commit_message>
fix column rigid column in table view
</commit_message>
<xml_diff>
--- a/001 Project/001 Application/sql/slowniki.xlsx
+++ b/001 Project/001 Application/sql/slowniki.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\001_programy\005_competitive\001 Project\001 Application\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{293F7667-E4CB-4B26-80B3-8260BF850140}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5869C1CF-D50D-4F34-BAD1-F93F62CB86F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{0A1D0093-9CB5-406E-8959-9EDFC34F9A2F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{0A1D0093-9CB5-406E-8959-9EDFC34F9A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sub Category uspojnienie" sheetId="1" r:id="rId1"/>
     <sheet name="Stacje" sheetId="2" r:id="rId2"/>
+    <sheet name="brand_uspione" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Stacje!$A$1:$C$917</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2945" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3029" uniqueCount="567">
   <si>
     <t>NIELSEN</t>
   </si>
@@ -1580,6 +1581,156 @@
   </si>
   <si>
     <t>TVN Media</t>
+  </si>
+  <si>
+    <t>Alfa romeo</t>
+  </si>
+  <si>
+    <t>Alfa Romeo</t>
+  </si>
+  <si>
+    <t>Audi</t>
+  </si>
+  <si>
+    <t>Auto cuby m&amp;p</t>
+  </si>
+  <si>
+    <t>Auto cuby</t>
+  </si>
+  <si>
+    <t>Bmw</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Bmw motorrad</t>
+  </si>
+  <si>
+    <t>Citroen</t>
+  </si>
+  <si>
+    <t>Dacia</t>
+  </si>
+  <si>
+    <t>Ducati motory</t>
+  </si>
+  <si>
+    <t>Ducati</t>
+  </si>
+  <si>
+    <t>Electromobility poland</t>
+  </si>
+  <si>
+    <t>Electromobility Poland</t>
+  </si>
+  <si>
+    <t>Fiat</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Harley-davidson</t>
+  </si>
+  <si>
+    <t>Harley-Davidson</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>Infiniti</t>
+  </si>
+  <si>
+    <t>Jaguar</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>Jodmet</t>
+  </si>
+  <si>
+    <t>Junak</t>
+  </si>
+  <si>
+    <t>Kia</t>
+  </si>
+  <si>
+    <t>Kia - eurosport</t>
+  </si>
+  <si>
+    <t>Land rover</t>
+  </si>
+  <si>
+    <t>Land Rover</t>
+  </si>
+  <si>
+    <t>Lexus</t>
+  </si>
+  <si>
+    <t>Mazda</t>
+  </si>
+  <si>
+    <t>Melex</t>
+  </si>
+  <si>
+    <t>Mercedes od 2008</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz</t>
+  </si>
+  <si>
+    <t>Mini</t>
+  </si>
+  <si>
+    <t>Mitsubishi</t>
+  </si>
+  <si>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Opel</t>
+  </si>
+  <si>
+    <t>Peugeot</t>
+  </si>
+  <si>
+    <t>Renault</t>
+  </si>
+  <si>
+    <t>Seat</t>
+  </si>
+  <si>
+    <t>Skoda</t>
+  </si>
+  <si>
+    <t>Suzuki</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Toyota motor poland</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>Yamaha motors</t>
+  </si>
+  <si>
+    <t>Yamaha</t>
+  </si>
+  <si>
+    <t>Zala</t>
   </si>
 </sst>
 </file>
@@ -2154,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4528EBFB-DB63-41B8-8FCC-2CE5B44EE30D}">
   <dimension ref="A1:C1451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1417" workbookViewId="0">
-      <selection activeCell="G1422" sqref="G1422"/>
+    <sheetView topLeftCell="A1417" workbookViewId="0">
+      <selection activeCell="F1434" sqref="F1434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18129,4 +18280,359 @@
   <autoFilter ref="A1:C917" xr:uid="{271BC1EA-87D8-454F-B1B1-655425F08199}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0F94EC-2897-4DEE-A08B-16BA6EFF1BAD}">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>566</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix function 'get data from columns' bug with NoneType
</commit_message>
<xml_diff>
--- a/001 Project/001 Application/sql/slowniki.xlsx
+++ b/001 Project/001 Application/sql/slowniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\001_programy\005_competitive\001 Project\001 Application\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5869C1CF-D50D-4F34-BAD1-F93F62CB86F9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D37AE6FE-4A5C-4289-A8F2-BEA37EEAD9EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{0A1D0093-9CB5-406E-8959-9EDFC34F9A2F}"/>
   </bookViews>
@@ -18287,7 +18287,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>